<commit_message>
Revised eeg data load
</commit_message>
<xml_diff>
--- a/Data/EEG Studies.xlsx
+++ b/Data/EEG Studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/EEG_ML_Pipeline/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC7C0EE-6814-8D44-9EAC-70515F7294D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7FD555-95A8-1D4F-AA74-A2FD23897955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16920" yWindow="6940" windowWidth="32380" windowHeight="18020" xr2:uid="{977EEC3C-A948-C04F-B7FA-E69A2E36C13C}"/>
   </bookViews>
@@ -641,7 +641,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Reorg and data download
</commit_message>
<xml_diff>
--- a/Data/EEG Studies.xlsx
+++ b/Data/EEG Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/EEG_ML_Pipeline/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7FD555-95A8-1D4F-AA74-A2FD23897955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9710A0F3-A40E-0641-9BA5-225BE259598E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="6940" windowWidth="32380" windowHeight="18020" xr2:uid="{977EEC3C-A948-C04F-B7FA-E69A2E36C13C}"/>
+    <workbookView xWindow="23300" yWindow="6940" windowWidth="32380" windowHeight="18020" xr2:uid="{977EEC3C-A948-C04F-B7FA-E69A2E36C13C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,10 +299,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,7 +641,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,11 +668,11 @@
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
@@ -821,7 +821,7 @@
       <c r="B16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>